<commit_message>
Added symbolic regression using Feyn
</commit_message>
<xml_diff>
--- a/input_data/strand_features_N50.xlsx
+++ b/input_data/strand_features_N50.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1950" windowWidth="29040" windowHeight="17520" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-1950" windowWidth="29040" windowHeight="17520" firstSheet="5" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Sequences" sheetId="11" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="Choice9" sheetId="15" r:id="rId15"/>
     <sheet name="Choice10" sheetId="16" r:id="rId16"/>
     <sheet name="Choice11" sheetId="17" r:id="rId17"/>
+    <sheet name="Choice13" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="54">
   <si>
     <t>ddG</t>
   </si>
@@ -3039,6 +3040,667 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:19" ht="78.75">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="5"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2">
+        <v>-17.77</v>
+      </c>
+      <c r="B2">
+        <v>26.729999999999997</v>
+      </c>
+      <c r="C2">
+        <v>9.33</v>
+      </c>
+      <c r="D2">
+        <v>7.86</v>
+      </c>
+      <c r="E2">
+        <v>7.86</v>
+      </c>
+      <c r="F2">
+        <v>8.66</v>
+      </c>
+      <c r="G2">
+        <v>16.059999999999999</v>
+      </c>
+      <c r="H2">
+        <v>2.5</v>
+      </c>
+      <c r="I2" s="4">
+        <v>3.0925E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3">
+        <v>-16.690000000000001</v>
+      </c>
+      <c r="B3">
+        <v>21.25</v>
+      </c>
+      <c r="C3">
+        <v>5.99</v>
+      </c>
+      <c r="D3">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E3">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>7.24</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>3.8952999999999998E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4">
+        <v>-16.350000000000001</v>
+      </c>
+      <c r="B4">
+        <v>18.34</v>
+      </c>
+      <c r="C4">
+        <v>7.3100000000000005</v>
+      </c>
+      <c r="D4">
+        <v>6.04</v>
+      </c>
+      <c r="E4">
+        <v>6.04</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>5.65</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>3.5540000000000002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5">
+        <v>-16</v>
+      </c>
+      <c r="B5">
+        <v>18.79</v>
+      </c>
+      <c r="C5">
+        <v>9.84</v>
+      </c>
+      <c r="D5">
+        <v>2.25</v>
+      </c>
+      <c r="E5">
+        <v>4.74</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="H5">
+        <v>7.65</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1.0139999999999999E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6">
+        <v>-15.79</v>
+      </c>
+      <c r="B6">
+        <v>21.18</v>
+      </c>
+      <c r="C6">
+        <v>14.89</v>
+      </c>
+      <c r="D6">
+        <v>13.74</v>
+      </c>
+      <c r="E6">
+        <v>13.74</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>16.07</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1.5604E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7">
+        <v>-15.25</v>
+      </c>
+      <c r="B7">
+        <v>18.479999999999997</v>
+      </c>
+      <c r="C7">
+        <v>11.13</v>
+      </c>
+      <c r="D7">
+        <v>5.21</v>
+      </c>
+      <c r="E7">
+        <v>5.21</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>9.61</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1.6971999999999999E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8">
+        <v>-15.09</v>
+      </c>
+      <c r="B8">
+        <v>14.25</v>
+      </c>
+      <c r="C8">
+        <v>7.43</v>
+      </c>
+      <c r="D8">
+        <v>3.22</v>
+      </c>
+      <c r="E8">
+        <v>5.01</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1.68</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2.2532E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9">
+        <v>-14.83</v>
+      </c>
+      <c r="B9">
+        <v>14.75</v>
+      </c>
+      <c r="C9">
+        <v>9.83</v>
+      </c>
+      <c r="D9">
+        <v>8.74</v>
+      </c>
+      <c r="E9">
+        <v>8.74</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>4.58</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1.3726999999999999E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10">
+        <v>-14.76</v>
+      </c>
+      <c r="B10">
+        <v>22.73</v>
+      </c>
+      <c r="C10">
+        <v>10.77</v>
+      </c>
+      <c r="D10">
+        <v>4.42</v>
+      </c>
+      <c r="E10">
+        <v>4.42</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>13.5</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>4.1723E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11">
+        <v>-14.6</v>
+      </c>
+      <c r="B11">
+        <v>15.35</v>
+      </c>
+      <c r="C11">
+        <v>6.3800000000000008</v>
+      </c>
+      <c r="D11">
+        <v>1.36</v>
+      </c>
+      <c r="E11">
+        <v>3.72</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1.73</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>6.4794000000000002E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12">
+        <v>-14.36</v>
+      </c>
+      <c r="B12">
+        <v>15.950000000000001</v>
+      </c>
+      <c r="C12">
+        <v>12.35</v>
+      </c>
+      <c r="D12">
+        <v>7.95</v>
+      </c>
+      <c r="E12">
+        <v>7.95</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>9.9786999999999999E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13">
+        <v>-14.36</v>
+      </c>
+      <c r="B13">
+        <v>15.419999999999998</v>
+      </c>
+      <c r="C13">
+        <v>18.260000000000002</v>
+      </c>
+      <c r="D13">
+        <v>19.190000000000001</v>
+      </c>
+      <c r="E13">
+        <v>19.190000000000001</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>13.68</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>6.4641999999999995E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14">
+        <v>-14.36</v>
+      </c>
+      <c r="B14">
+        <v>18.87</v>
+      </c>
+      <c r="C14">
+        <v>16.79</v>
+      </c>
+      <c r="D14">
+        <v>8.08</v>
+      </c>
+      <c r="E14">
+        <v>8.08</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>15.66</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>5.2469000000000002E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15">
+        <v>-14.2</v>
+      </c>
+      <c r="B15">
+        <v>13.34</v>
+      </c>
+      <c r="C15">
+        <v>9.64</v>
+      </c>
+      <c r="D15">
+        <v>5.18</v>
+      </c>
+      <c r="E15">
+        <v>5.18</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>2.98</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>4.4014999999999998E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16">
+        <v>-14.14</v>
+      </c>
+      <c r="B16">
+        <v>14.82</v>
+      </c>
+      <c r="C16">
+        <v>9.58</v>
+      </c>
+      <c r="D16">
+        <v>6.11</v>
+      </c>
+      <c r="E16">
+        <v>6.11</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H16">
+        <v>3.26</v>
+      </c>
+      <c r="I16" s="4">
+        <v>5.1549999999999999E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>-14.12</v>
+      </c>
+      <c r="B17">
+        <v>14.189999999999998</v>
+      </c>
+      <c r="C17">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D17">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E17">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="F17">
+        <v>0.87</v>
+      </c>
+      <c r="G17">
+        <v>11.79</v>
+      </c>
+      <c r="H17">
+        <v>4.32</v>
+      </c>
+      <c r="I17" s="4">
+        <v>1.0442000000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>-14</v>
+      </c>
+      <c r="B18">
+        <v>17.829999999999998</v>
+      </c>
+      <c r="C18">
+        <v>15.93</v>
+      </c>
+      <c r="D18">
+        <v>4.47</v>
+      </c>
+      <c r="E18">
+        <v>4.47</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>13.76</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>1.5133000000000001E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>-13.89</v>
+      </c>
+      <c r="B19">
+        <v>15.26</v>
+      </c>
+      <c r="C19">
+        <v>13.4</v>
+      </c>
+      <c r="D19">
+        <v>7.96</v>
+      </c>
+      <c r="E19">
+        <v>7.96</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>8.66</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>9.4930000000000001E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>-13.88</v>
+      </c>
+      <c r="B20">
+        <v>15.18</v>
+      </c>
+      <c r="C20">
+        <v>17.82</v>
+      </c>
+      <c r="D20">
+        <v>18.72</v>
+      </c>
+      <c r="E20">
+        <v>18.72</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>13</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>5.7309000000000003E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>-13.12</v>
+      </c>
+      <c r="B21">
+        <v>11.57</v>
+      </c>
+      <c r="C21">
+        <v>13.01</v>
+      </c>
+      <c r="D21">
+        <v>7.62</v>
+      </c>
+      <c r="E21">
+        <v>7.62</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>4.58</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>7.2818000000000007E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>-13.02</v>
+      </c>
+      <c r="B22">
+        <v>14.09</v>
+      </c>
+      <c r="C22">
+        <v>12.440000000000001</v>
+      </c>
+      <c r="D22">
+        <v>7.67</v>
+      </c>
+      <c r="E22">
+        <v>7.67</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>6.53</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>7.8464E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
@@ -3304,7 +3966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -5719,7 +6381,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+      <selection activeCell="N1" activeCellId="8" sqref="A1:A1048576 B1:B1048576 C1:C1048576 D1:D1048576 E1:E1048576 H1:H1048576 I1:I1048576 M1:M1048576 N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>